<commit_message>
updating with better translations of first Amua case study
</commit_message>
<xml_diff>
--- a/case-studies/answer-keys/cs1_PE_v1_ANS.xlsx
+++ b/case-studies/answer-keys/cs1_PE_v1_ANS.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/answer-keys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94DE28C-43D2-6343-997F-7AB262874FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6BD596-875E-8B40-AFE2-D6FC9A9ABD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33160" windowHeight="23320" activeTab="2" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" activeTab="1" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="parameters" sheetId="3" r:id="rId1"/>
-    <sheet name="Decision Tree" sheetId="1" r:id="rId2"/>
-    <sheet name="Summary" sheetId="4" r:id="rId3"/>
+    <sheet name="parámetros" sheetId="3" r:id="rId1"/>
+    <sheet name="Árbol de decisión" sheetId="1" r:id="rId2"/>
+    <sheet name="Resumen" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="c_ac">parameters!$B$10</definedName>
-    <definedName name="c_fatal_pe_or_hem">parameters!$B$8</definedName>
-    <definedName name="c_healthy">parameters!$B$9</definedName>
-    <definedName name="c_pe">parameters!$B$7</definedName>
-    <definedName name="N_pop">parameters!$B$2</definedName>
-    <definedName name="p_fatal_bleed_with_ac">parameters!$B$5</definedName>
-    <definedName name="p_fatal_recurrent_pe">parameters!$B$6</definedName>
-    <definedName name="p_fatal_recurrent_pe_with_ac">parameters!$B$4</definedName>
-    <definedName name="p_pe">parameters!$B$3</definedName>
-    <definedName name="u_healthy">parameters!#REF!</definedName>
+    <definedName name="c_ac">parámetros!$B$10</definedName>
+    <definedName name="c_fatal_pe_or_hem">parámetros!$B$8</definedName>
+    <definedName name="c_healthy">parámetros!$B$9</definedName>
+    <definedName name="c_pe">parámetros!$B$7</definedName>
+    <definedName name="N_pop">parámetros!$B$2</definedName>
+    <definedName name="p_fatal_bleed_with_ac">parámetros!$B$5</definedName>
+    <definedName name="p_fatal_recurrent_pe">parámetros!$B$6</definedName>
+    <definedName name="p_fatal_recurrent_pe_with_ac">parámetros!$B$4</definedName>
+    <definedName name="p_pe">parámetros!$B$3</definedName>
+    <definedName name="u_healthy">parámetros!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,10 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
-  <si>
-    <t>Suspected PE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>param</t>
   </si>
@@ -76,18 +73,12 @@
     <t>p_fatal_recurrent_pe_with_ac</t>
   </si>
   <si>
-    <t>Probability of recurrent PE leading to fatal bleed/hemmorhage WITH anti-coagulant</t>
-  </si>
-  <si>
     <t>Probability of fatal bleed due WITH anti-coagulant</t>
   </si>
   <si>
     <t>p_fatal_recurrent_pe</t>
   </si>
   <si>
-    <t>Probability of recurrent PE leading to fatal bleed/hemmorhage with no anti-coagulant</t>
-  </si>
-  <si>
     <t>c_healthy</t>
   </si>
   <si>
@@ -106,45 +97,12 @@
     <t>Population size</t>
   </si>
   <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>No PE</t>
-  </si>
-  <si>
     <t>Survive</t>
   </si>
   <si>
-    <t>Dead</t>
-  </si>
-  <si>
-    <t>Fatal Hem</t>
-  </si>
-  <si>
-    <t>No PE, AC</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>Survive, No AC</t>
-  </si>
-  <si>
-    <t>PE, No AC</t>
-  </si>
-  <si>
-    <t>Anticoagulant</t>
-  </si>
-  <si>
-    <t>No Anti-coagulant</t>
-  </si>
-  <si>
-    <t>Die</t>
-  </si>
-  <si>
-    <t>PE + AC</t>
-  </si>
-  <si>
     <t>Outcome</t>
   </si>
   <si>
@@ -160,31 +118,83 @@
     <t>Effectiveness (Survival)</t>
   </si>
   <si>
-    <t>Expected Survival</t>
-  </si>
-  <si>
-    <t>Expected Costs</t>
-  </si>
-  <si>
-    <t>Anti-coagulant therapy</t>
-  </si>
-  <si>
-    <t>No Anti-coagulant therapy</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>Expected Deaths (number)</t>
-  </si>
-  <si>
-    <t>Fatal PE</t>
-  </si>
-  <si>
     <t>Cost of fatal PE</t>
   </si>
   <si>
-    <t>AC costs</t>
+    <t>Probability of recurrent fatal PE WITH anti-coagulant</t>
+  </si>
+  <si>
+    <t>Probability of recurrent fatal PE with no anti-coagulant</t>
+  </si>
+  <si>
+    <t>Sospecha de EP</t>
+  </si>
+  <si>
+    <t>Anticoagulante</t>
+  </si>
+  <si>
+    <t>No Anticoagulante</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>No EP</t>
+  </si>
+  <si>
+    <t>EP mortal</t>
+  </si>
+  <si>
+    <t>Sobrevivir</t>
+  </si>
+  <si>
+    <t>Hemorragia mortal</t>
+  </si>
+  <si>
+    <t>Muertos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EP + AC </t>
+  </si>
+  <si>
+    <t>No EP, AC</t>
+  </si>
+  <si>
+    <t>EP, No AC</t>
+  </si>
+  <si>
+    <t>Sobrevivir, No AC</t>
+  </si>
+  <si>
+    <t>Estrategia</t>
+  </si>
+  <si>
+    <t>Costos previstos</t>
+  </si>
+  <si>
+    <t>Supervivencia prevista</t>
+  </si>
+  <si>
+    <t>Muertes previstas (número)</t>
+  </si>
+  <si>
+    <t>No Terapia anticoagulantetherapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terapia anticoagulante
+</t>
+  </si>
+  <si>
+    <t>Tenga en cuenta lo siguiente:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En esta clave de respuestas, hemos ignorado estos costes, pero podría </t>
+  </si>
+  <si>
+    <t xml:space="preserve">incluirlos para el 19% de los individuos de cada brazo que experimentan el evento PE inicial. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El texto del estudio de caso no deja muy claro el coste del evento inicial de EP (5.000). </t>
   </si>
 </sst>
 </file>
@@ -195,7 +205,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,6 +231,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -373,10 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -387,21 +400,28 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1078,7 +1098,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,113 +1111,113 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4">
         <v>100000</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>0.19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>0.05</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
         <v>0.04</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>0.25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <f>5000</f>
         <v>5000</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4">
         <v>10000</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4">
         <v>1000</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1210,10 +1230,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="C1:R53"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,28 +1258,37 @@
     <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:18" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="N1" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="12"/>
       <c r="R1" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="6:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>47</v>
+      </c>
       <c r="N2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="6:18" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L3" s="22" t="s">
-        <v>42</v>
+    <row r="3" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -1267,23 +1296,26 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="6:18" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L4" s="22"/>
+    <row r="4" spans="1:18" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="20"/>
       <c r="M4" s="6"/>
       <c r="N4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="15">
-        <f>c_pe + c_fatal_pe_or_hem+c_ac</f>
-        <v>16000</v>
+        <f xml:space="preserve"> c_fatal_pe_or_hem+c_ac</f>
+        <v>11000</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L5" s="8">
         <f>p_fatal_recurrent_pe_with_ac</f>
         <v>0.05</v>
@@ -1294,58 +1326,58 @@
       <c r="Q5" s="11"/>
       <c r="R5" s="14"/>
     </row>
-    <row r="6" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="6"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="6:18" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I8" s="22" t="s">
-        <v>18</v>
+    <row r="8" spans="1:18" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="6:18" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I9" s="22"/>
+    <row r="9" spans="1:18" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="20"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I10" s="8">
         <f>p_pe</f>
         <v>0.19</v>
       </c>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I11" s="7"/>
-      <c r="L11" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="6:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="22" t="s">
-        <v>27</v>
+      <c r="L11" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="L12" s="24"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="6"/>
       <c r="N12" s="15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="15">
-        <f>c_pe + c_ac+c_healthy</f>
-        <v>6000</v>
+        <f xml:space="preserve"> c_ac+c_healthy</f>
+        <v>1000</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="R12" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="6:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="22"/>
+    <row r="13" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="20"/>
       <c r="G13" s="6"/>
       <c r="I13" s="7"/>
       <c r="L13" s="8">
@@ -1358,28 +1390,28 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="F14" s="22"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F14" s="20"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="6:18" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="L16" s="22" t="s">
-        <v>22</v>
+      <c r="L16" s="20" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="3:18" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="L17" s="22"/>
+      <c r="L17" s="20"/>
       <c r="M17" s="6"/>
       <c r="N17" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="15">
@@ -1393,8 +1425,8 @@
     </row>
     <row r="18" spans="3:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="7"/>
-      <c r="I18" s="22" t="s">
-        <v>19</v>
+      <c r="I18" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="L18" s="8">
         <f>p_fatal_bleed_with_ac</f>
@@ -1408,7 +1440,7 @@
     </row>
     <row r="19" spans="3:18" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F19" s="7"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="21"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.2">
@@ -1430,16 +1462,16 @@
     </row>
     <row r="23" spans="3:18" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F23" s="7"/>
-      <c r="L23" s="22" t="s">
-        <v>20</v>
+      <c r="L23" s="20" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="3:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F24" s="7"/>
-      <c r="L24" s="24"/>
+      <c r="L24" s="21"/>
       <c r="M24" s="6"/>
       <c r="N24" s="15" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="P24" s="15">
         <f>c_ac+c_healthy</f>
@@ -1451,7 +1483,7 @@
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="F25" s="23"/>
+      <c r="F25" s="25"/>
       <c r="L25" s="8">
         <f>1-p_fatal_bleed_with_ac</f>
         <v>0.96</v>
@@ -1462,23 +1494,23 @@
       <c r="R25" s="14"/>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="F26" s="23"/>
+      <c r="F26" s="25"/>
     </row>
     <row r="27" spans="3:18" x14ac:dyDescent="0.2">
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C28" s="22" t="s">
-        <v>0</v>
+      <c r="C28" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="D28" s="6"/>
       <c r="F28" s="7"/>
-      <c r="L28" s="27"/>
+      <c r="L28" s="24"/>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C29" s="22"/>
+      <c r="C29" s="20"/>
       <c r="F29" s="7"/>
-      <c r="L29" s="27"/>
+      <c r="L29" s="24"/>
       <c r="N29" s="14"/>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.2">
@@ -1487,20 +1519,20 @@
     </row>
     <row r="31" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F31" s="7"/>
-      <c r="L31" s="22" t="s">
-        <v>42</v>
+      <c r="L31" s="20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F32" s="7"/>
-      <c r="L32" s="22"/>
+      <c r="L32" s="20"/>
       <c r="M32" s="6"/>
       <c r="N32" s="15" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="P32" s="15">
-        <f>c_pe + c_fatal_pe_or_hem</f>
-        <v>15000</v>
+        <f>c_fatal_pe_or_hem</f>
+        <v>10000</v>
       </c>
       <c r="Q32" s="11"/>
       <c r="R32" s="15">
@@ -1525,14 +1557,14 @@
     </row>
     <row r="35" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F35" s="7"/>
-      <c r="I35" s="22" t="s">
-        <v>18</v>
+      <c r="I35" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="L35" s="7"/>
     </row>
     <row r="36" spans="6:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F36" s="7"/>
-      <c r="I36" s="22"/>
+      <c r="I36" s="20"/>
       <c r="L36" s="7"/>
     </row>
     <row r="37" spans="6:18" x14ac:dyDescent="0.2">
@@ -1546,23 +1578,23 @@
     <row r="38" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="L38" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F39" s="22" t="s">
-        <v>28</v>
+      <c r="L38" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="6:18" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="L39" s="24"/>
+      <c r="L39" s="21"/>
       <c r="M39" s="6"/>
       <c r="N39" s="15" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="P39" s="15">
-        <f>c_pe</f>
-        <v>5000</v>
+        <f>c_healthy</f>
+        <v>0</v>
       </c>
       <c r="Q39" s="11"/>
       <c r="R39" s="15">
@@ -1570,7 +1602,7 @@
       </c>
     </row>
     <row r="40" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="F40" s="22"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="6"/>
       <c r="I40" s="7"/>
       <c r="L40" s="8">
@@ -1583,7 +1615,7 @@
       <c r="R40" s="14"/>
     </row>
     <row r="41" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="F41" s="24"/>
+      <c r="F41" s="21"/>
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="6:18" x14ac:dyDescent="0.2">
@@ -1592,23 +1624,23 @@
     </row>
     <row r="43" spans="6:18" x14ac:dyDescent="0.2">
       <c r="I43" s="7"/>
-      <c r="L43" s="25"/>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" spans="6:18" x14ac:dyDescent="0.2">
       <c r="I44" s="7"/>
-      <c r="L44" s="25"/>
+      <c r="L44" s="22"/>
       <c r="N44" s="14"/>
     </row>
     <row r="45" spans="6:18" x14ac:dyDescent="0.2">
-      <c r="I45" s="22" t="s">
-        <v>19</v>
+      <c r="I45" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="N45" s="14"/>
     </row>
     <row r="46" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="24"/>
-      <c r="L46" s="25" t="s">
-        <v>20</v>
+      <c r="I46" s="21"/>
+      <c r="L46" s="22" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="6:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1618,10 +1650,10 @@
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
-      <c r="L47" s="26"/>
+      <c r="L47" s="23"/>
       <c r="M47" s="6"/>
       <c r="N47" s="15" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="P47" s="15">
         <f>c_healthy</f>
@@ -1639,13 +1671,23 @@
       <c r="R48" s="14"/>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F52" s="25"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F53" s="25"/>
+      <c r="F53" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L43:L44"/>
     <mergeCell ref="I45:I46"/>
     <mergeCell ref="L46:L47"/>
     <mergeCell ref="F52:F53"/>
@@ -1654,16 +1696,6 @@
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="L31:L32"/>
     <mergeCell ref="F39:F41"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L23:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1674,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110C7B89-70E6-0640-AD1A-EE76B2818E1A}">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="197" zoomScaleNormal="197" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="197" zoomScaleNormal="197" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1686,65 +1718,62 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="17">
-        <f>'Decision Tree'!P4*'Decision Tree'!L5*'Decision Tree'!I10+'Decision Tree'!P12*'Decision Tree'!L13*'Decision Tree'!I10+'Decision Tree'!P17*'Decision Tree'!L18*'Decision Tree'!I20+'Decision Tree'!P24*'Decision Tree'!L25*'Decision Tree'!I20</f>
-        <v>2369</v>
-      </c>
-      <c r="D3" s="16">
-        <f>'Decision Tree'!R4*'Decision Tree'!L5*'Decision Tree'!I10+'Decision Tree'!R12*'Decision Tree'!L13*'Decision Tree'!I10+'Decision Tree'!R17*'Decision Tree'!L18*'Decision Tree'!I20+'Decision Tree'!R24*'Decision Tree'!L25*'Decision Tree'!I20</f>
+    <row r="3" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="27">
+        <f>'Árbol de decisión'!P4*'Árbol de decisión'!L5*'Árbol de decisión'!I10+'Árbol de decisión'!P12*'Árbol de decisión'!L13*'Árbol de decisión'!I10+'Árbol de decisión'!P17*'Árbol de decisión'!L18*'Árbol de decisión'!I20+'Árbol de decisión'!P24*'Árbol de decisión'!L25*'Árbol de decisión'!I20</f>
+        <v>1419</v>
+      </c>
+      <c r="D3" s="11">
+        <f>'Árbol de decisión'!R4*'Árbol de decisión'!L5*'Árbol de decisión'!I10+'Árbol de decisión'!R12*'Árbol de decisión'!L13*'Árbol de decisión'!I10+'Árbol de decisión'!R17*'Árbol de decisión'!L18*'Árbol de decisión'!I20+'Árbol de decisión'!R24*'Árbol de decisión'!L25*'Árbol de decisión'!I20</f>
         <v>0.95810000000000006</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="27">
         <f>N_pop*(1-D3)</f>
         <v>4189.9999999999936</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="17">
-        <f>'Decision Tree'!P32*'Decision Tree'!L33*'Decision Tree'!I37+'Decision Tree'!P39*'Decision Tree'!L40*'Decision Tree'!I37+'Decision Tree'!P47*'Decision Tree'!I47</f>
-        <v>1425</v>
-      </c>
-      <c r="D4" s="16">
-        <f>'Decision Tree'!R32*'Decision Tree'!L33*'Decision Tree'!I37+'Decision Tree'!R39*'Decision Tree'!L40*'Decision Tree'!I37+'Decision Tree'!R47*'Decision Tree'!I47</f>
+        <v>42</v>
+      </c>
+      <c r="C4" s="27">
+        <f>'Árbol de decisión'!P32*'Árbol de decisión'!L33*'Árbol de decisión'!I37+'Árbol de decisión'!P39*'Árbol de decisión'!L40*'Árbol de decisión'!I37+'Árbol de decisión'!P47*'Árbol de decisión'!I47</f>
+        <v>475</v>
+      </c>
+      <c r="D4" s="11">
+        <f>'Árbol de decisión'!R32*'Árbol de decisión'!L33*'Árbol de decisión'!I37+'Árbol de decisión'!R39*'Árbol de decisión'!L40*'Árbol de decisión'!I37+'Árbol de decisión'!R47*'Árbol de decisión'!I47</f>
         <v>0.95250000000000012</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="27">
         <f>N_pop*(1-D4)</f>
         <v>4749.9999999999873</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="21"/>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1">
-        <f>(0.19*0.01*16000) + (0.19*0.99*6000) + (0.81*0.008*11000) + (0.81*0.992*1000)</f>
-        <v>2033.8</v>
-      </c>
+      <c r="B7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commiting again afater a website snafu
</commit_message>
<xml_diff>
--- a/case-studies/answer-keys/cs1_PE_v1_ANS.xlsx
+++ b/case-studies/answer-keys/cs1_PE_v1_ANS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/answer-keys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6BD596-875E-8B40-AFE2-D6FC9A9ABD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA37EFA-57DF-264F-BEC9-8FABAB89EA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" activeTab="1" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" xr2:uid="{199646B0-E4D7-5E4D-B717-C3E52A2D89BD}"/>
   </bookViews>
   <sheets>
     <sheet name="parámetros" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>param</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Probability of recurrent fatal PE with no anti-coagulant</t>
+  </si>
+  <si>
+    <t>Probabilidad de EP mortal recurrente CON anticoagulante</t>
   </si>
   <si>
     <t>Sospecha de EP</t>
@@ -195,6 +198,30 @@
   </si>
   <si>
     <t xml:space="preserve">El texto del estudio de caso no deja muy claro el coste del evento inicial de EP (5.000). </t>
+  </si>
+  <si>
+    <t>Tamaño de la población</t>
+  </si>
+  <si>
+    <t>Probabilidad de embolia pulmonar</t>
+  </si>
+  <si>
+    <t>Probabilidad de hemorragia mortal con anticoagulante</t>
+  </si>
+  <si>
+    <t>Probabilidad de EP mortal recurrente sin anticoagulante</t>
+  </si>
+  <si>
+    <t>Costo de la EP no mortal</t>
+  </si>
+  <si>
+    <t>Costo de la EP mortal</t>
+  </si>
+  <si>
+    <t>Costo del estado de salud perfecta</t>
+  </si>
+  <si>
+    <t>Costo del anticoagulante</t>
   </si>
 </sst>
 </file>
@@ -1095,21 +1122,22 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="97.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="52.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1119,8 +1147,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1128,10 +1159,13 @@
         <v>100000</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1139,10 +1173,13 @@
         <v>0.19</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1150,10 +1187,13 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1161,10 +1201,13 @@
         <v>0.04</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1172,10 +1215,13 @@
         <v>0.25</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1184,10 +1230,13 @@
         <v>5000</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1195,10 +1244,13 @@
         <v>10000</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1206,10 +1258,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1217,6 +1272,9 @@
         <v>1000</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1232,7 +1290,7 @@
   </sheetPr>
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+    <sheetView zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -1260,7 +1318,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>17</v>
@@ -1276,7 +1334,7 @@
     </row>
     <row r="2" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N2" s="3"/>
       <c r="P2" s="3"/>
@@ -1285,10 +1343,10 @@
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -1298,12 +1356,12 @@
     </row>
     <row r="4" spans="1:18" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="6"/>
       <c r="N4" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="15">
@@ -1335,7 +1393,7 @@
     </row>
     <row r="8" spans="1:18" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I8" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L8" s="7"/>
     </row>
@@ -1353,18 +1411,18 @@
     <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I11" s="7"/>
       <c r="L11" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I12" s="7"/>
       <c r="L12" s="21"/>
       <c r="M12" s="6"/>
       <c r="N12" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="15">
@@ -1402,7 +1460,7 @@
       <c r="F16" s="7"/>
       <c r="I16" s="7"/>
       <c r="L16" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="3:18" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1411,7 +1469,7 @@
       <c r="L17" s="20"/>
       <c r="M17" s="6"/>
       <c r="N17" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="15">
@@ -1426,7 +1484,7 @@
     <row r="18" spans="3:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="7"/>
       <c r="I18" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L18" s="8">
         <f>p_fatal_bleed_with_ac</f>
@@ -1463,7 +1521,7 @@
     <row r="23" spans="3:18" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F23" s="7"/>
       <c r="L23" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="3:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1471,7 +1529,7 @@
       <c r="L24" s="21"/>
       <c r="M24" s="6"/>
       <c r="N24" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P24" s="15">
         <f>c_ac+c_healthy</f>
@@ -1501,7 +1559,7 @@
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C28" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28" s="6"/>
       <c r="F28" s="7"/>
@@ -1520,7 +1578,7 @@
     <row r="31" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F31" s="7"/>
       <c r="L31" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="3:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1528,7 +1586,7 @@
       <c r="L32" s="20"/>
       <c r="M32" s="6"/>
       <c r="N32" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P32" s="15">
         <f>c_fatal_pe_or_hem</f>
@@ -1558,7 +1616,7 @@
     <row r="35" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F35" s="7"/>
       <c r="I35" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L35" s="7"/>
     </row>
@@ -1579,18 +1637,18 @@
       <c r="F38" s="7"/>
       <c r="I38" s="7"/>
       <c r="L38" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="6:18" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F39" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I39" s="7"/>
       <c r="L39" s="21"/>
       <c r="M39" s="6"/>
       <c r="N39" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P39" s="15">
         <f>c_healthy</f>
@@ -1633,7 +1691,7 @@
     </row>
     <row r="45" spans="6:18" x14ac:dyDescent="0.2">
       <c r="I45" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N45" s="14"/>
     </row>
@@ -1653,7 +1711,7 @@
       <c r="L47" s="23"/>
       <c r="M47" s="6"/>
       <c r="N47" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P47" s="15">
         <f>c_healthy</f>
@@ -1720,21 +1778,21 @@
   <sheetData>
     <row r="2" spans="2:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B2" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="27">
         <f>'Árbol de decisión'!P4*'Árbol de decisión'!L5*'Árbol de decisión'!I10+'Árbol de decisión'!P12*'Árbol de decisión'!L13*'Árbol de decisión'!I10+'Árbol de decisión'!P17*'Árbol de decisión'!L18*'Árbol de decisión'!I20+'Árbol de decisión'!P24*'Árbol de decisión'!L25*'Árbol de decisión'!I20</f>
@@ -1751,7 +1809,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="27">
         <f>'Árbol de decisión'!P32*'Árbol de decisión'!L33*'Árbol de decisión'!I37+'Árbol de decisión'!P39*'Árbol de decisión'!L40*'Árbol de decisión'!I37+'Árbol de decisión'!P47*'Árbol de decisión'!I47</f>

</xml_diff>